<commit_message>
Entrega do testes 19/04/2018
</commit_message>
<xml_diff>
--- a/grupo9/Casos_de_Testes_Grupo_9_validado_grupo_8.xlsx
+++ b/grupo9/Casos_de_Testes_Grupo_9_validado_grupo_8.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="28">
   <si>
     <t>Entrada (Salário bruto; Qtde de dependentes)</t>
   </si>
@@ -433,10 +433,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D12"/>
+  <dimension ref="A1:D20"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C5" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="D13" sqref="D13"/>
+    <sheetView tabSelected="1" topLeftCell="C11" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="D20" sqref="D20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -572,6 +572,11 @@
         <v>27</v>
       </c>
     </row>
+    <row r="20" spans="4:4" x14ac:dyDescent="0.2">
+      <c r="D20" t="s">
+        <v>24</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.74791666666666701" right="0.74791666666666701" top="0.98402777777777795" bottom="0.98402777777777795" header="0.51180555555555496" footer="0.51180555555555496"/>
   <pageSetup paperSize="0" scale="0" firstPageNumber="0" orientation="portrait" usePrinterDefaults="0" horizontalDpi="0" verticalDpi="0" copies="0"/>

</xml_diff>